<commit_message>
Update README and BOM
</commit_message>
<xml_diff>
--- a/ArduinoProMini_IOShield_BOM.xlsx
+++ b/ArduinoProMini_IOShield_BOM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
-  <si>
-    <t xml:space="preserve">Arduino Pro Mini IO Shield – BOM</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -191,6 +188,15 @@
   </si>
   <si>
     <t xml:space="preserve">J10, J11, J12, J13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mini 55 Points Breadboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiny 5x11 pin (55 points) Mini Breadboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aliexpress.com/item/7Pcs-Mini-55-Points-Breadboard-Solderless-Prototype-Tie-point-For-Arduino-GM/32670910749.html</t>
   </si>
 </sst>
 </file>
@@ -200,11 +206,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -223,17 +230,10 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="36"/>
-      <color rgb="FF804C19"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -324,16 +324,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,11 +365,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,7 +444,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF804C19"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -454,7 +458,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -465,300 +469,312 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.92"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="43.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="B5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="E14" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
V0.2: Add power soldering connection, add altenative ProMini pinout, move ICSP header; Add pictures;
</commit_message>
<xml_diff>
--- a/ArduinoProMini_IOShield_BOM.xlsx
+++ b/ArduinoProMini_IOShield_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">J0</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.aliexpress.com/item/100PCS-LOT-High-Quality-DC-Jack-DC-005-2-0-DC005-Power-Socket-5-5mm-2/32394200270.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">M7 / 1N4007</t>
   </si>
   <si>
@@ -68,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aliexpress.com/item/7-kinds-10pcs-70pcs-lot-SMD-diode-package-M1-1N4001-M4-1N4004-M7-1N4007-SS14-US1M/32774058057.html</t>
   </si>
   <si>
     <t xml:space="preserve">100µF</t>
@@ -460,8 +466,8 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,7 +477,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -521,44 +527,48 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -570,16 +580,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -591,19 +601,19 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -613,11 +623,11 @@
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -629,16 +639,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -650,19 +660,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -671,19 +681,19 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
       <c r="B10" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -692,19 +702,19 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -714,14 +724,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -731,11 +741,11 @@
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -746,13 +756,13 @@
       <c r="A14" s="6"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -762,10 +772,10 @@
     <row r="15" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
       <c r="B15" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -773,7 +783,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>